<commit_message>
Update vanwege 25e toets (dus nu 26 toetsmodules met menu-knop)
</commit_message>
<xml_diff>
--- a/Elektronica/Controller pin-toewijzingen.xlsx
+++ b/Elektronica/Controller pin-toewijzingen.xlsx
@@ -203,9 +203,6 @@
     <t>Shift</t>
   </si>
   <si>
-    <t>Menu</t>
-  </si>
-  <si>
     <t>Nog testen</t>
   </si>
   <si>
@@ -221,13 +218,16 @@
     <t>BatMon</t>
   </si>
   <si>
-    <t>SH/LDn1</t>
-  </si>
-  <si>
-    <t>SH/LDn2</t>
-  </si>
-  <si>
-    <t>SH/LDn3</t>
+    <t>SH/LDn</t>
+  </si>
+  <si>
+    <t>Tmenu</t>
+  </si>
+  <si>
+    <t>T25</t>
+  </si>
+  <si>
+    <t>NC</t>
   </si>
 </sst>
 </file>
@@ -321,7 +321,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -353,13 +353,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -745,16 +751,16 @@
       <c r="E4" s="10">
         <v>37</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>62</v>
+      <c r="F4" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="9" t="s">
-        <v>68</v>
+      <c r="A5" s="14" t="s">
+        <v>67</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>61</v>
@@ -773,11 +779,11 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>69</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>61</v>
       </c>
       <c r="C6" s="10">
         <v>17</v>
@@ -786,18 +792,18 @@
         <v>39</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>61</v>
+      <c r="B7" s="14" t="s">
+        <v>70</v>
       </c>
       <c r="C7" s="10">
         <v>2</v>
@@ -814,7 +820,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>55</v>
@@ -936,36 +942,36 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="14"/>
+      <c r="A17" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="15"/>
       <c r="C17" s="10" t="s">
         <v>50</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="15"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="15"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="9" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18" s="15"/>
+      <c r="F18" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1007,23 +1013,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="11.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="D1" s="13" t="s">
+      <c r="B1" s="17"/>
+      <c r="D1" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="J1" s="13" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="J1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">

</xml_diff>